<commit_message>
Saved 50% mixing XS and modified the current mixture in spreadsheet
</commit_message>
<xml_diff>
--- a/Miscellaneous/XSmixing.xlsx
+++ b/Miscellaneous/XSmixing.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarog\dissertation\Miscellaneous\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,9 +68,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -75,6 +81,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -123,7 +132,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -156,9 +165,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,6 +217,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -367,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="B32:H45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>1.5792999999999999E-5</v>
       </c>
@@ -668,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>3.3715999999999998E-4</v>
       </c>
@@ -682,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>1.9406E-3</v>
       </c>
@@ -696,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>5.7416000000000003E-3</v>
       </c>
@@ -710,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>1.5001E-2</v>
       </c>
@@ -724,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>3.7239000000000001E-2</v>
       </c>
@@ -738,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>4.4477700000000002E-2</v>
       </c>
@@ -761,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>0.1134</v>
       </c>
@@ -784,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>7.2347000000000004E-4</v>
       </c>
@@ -807,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>3.7498999999999999E-6</v>
       </c>
@@ -830,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>5.3184000000000002E-8</v>
       </c>
@@ -853,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>0</v>
       </c>
@@ -876,7 +919,7 @@
         <v>0.13244</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>0</v>
       </c>
@@ -899,24 +942,27 @@
         <v>2.4807000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="1">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.125</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1">
         <f>$B$31*B1+(1-$B$31)*B16</f>
-        <v>1.4289374999999999E-3</v>
+        <v>7.390312500000001E-4</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ref="C32:H32" si="0">$B$31*C1+(1-$B$31)*C16</f>
+        <f t="shared" ref="C32:E32" si="0">$B$31*C1+(1-$B$31)*C16</f>
         <v>0</v>
       </c>
       <c r="D32" s="1">
@@ -930,11 +976,23 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>1.1529750000000001E-3</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
-        <f t="shared" ref="B33:H33" si="1">$B$31*B2+(1-$B$31)*B17</f>
-        <v>6.27562825E-3</v>
+        <f t="shared" ref="B33:E33" si="1">$B$31*B2+(1-$B$31)*B17</f>
+        <v>1.059098875E-3</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
@@ -951,11 +1009,23 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>4.1890165E-3</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
-        <f t="shared" ref="B34:H34" si="2">$B$31*B3+(1-$B$31)*B18</f>
-        <v>6.2926865000000012E-2</v>
+        <f t="shared" ref="B34:E34" si="2">$B$31*B3+(1-$B$31)*B18</f>
+        <v>1.07687775E-2</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="2"/>
@@ -972,11 +1042,23 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>4.2063630000000005E-2</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
-        <f t="shared" ref="B35:H35" si="3">$B$31*B4+(1-$B$31)*B19</f>
-        <v>0.29883290000000001</v>
+        <f t="shared" ref="B35:E35" si="3">$B$31*B4+(1-$B$31)*B19</f>
+        <v>5.142265E-2</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="3"/>
@@ -993,11 +1075,23 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>0.19986880000000001</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <f t="shared" ref="B36:H36" si="4">$B$31*B5+(1-$B$31)*B20</f>
-        <v>0.52550764999999999</v>
+        <f t="shared" ref="B36:E36" si="4">$B$31*B5+(1-$B$31)*B20</f>
+        <v>9.2369275000000001E-2</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="4"/>
@@ -1014,11 +1108,23 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>0.35225230000000002</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <f t="shared" ref="B37:H37" si="5">$B$31*B6+(1-$B$31)*B21</f>
-        <v>0.7008812499999999</v>
+        <f t="shared" ref="B37:E37" si="5">$B$31*B6+(1-$B$31)*B21</f>
+        <v>0.12931437500000001</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="5"/>
@@ -1035,11 +1141,23 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>0.47225450000000002</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <f t="shared" ref="B38:H38" si="6">$B$31*B7+(1-$B$31)*B22</f>
-        <v>0.89307975000000006</v>
+        <f t="shared" ref="B38:E38" si="6">$B$31*B7+(1-$B$31)*B22</f>
+        <v>0.179879125</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="6"/>
@@ -1056,11 +1174,23 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>0.60779950000000005</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <f t="shared" ref="B39:H39" si="7">$B$31*B8+(1-$B$31)*B23</f>
-        <v>0.13904167499999998</v>
+        <v>6.0238362500000003E-2</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" si="7"/>
@@ -1086,15 +1216,36 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>0.10752035</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <f t="shared" ref="B40:H40" si="8">$B$31*B9+(1-$B$31)*B24</f>
-        <v>6.1650900000000002E-2</v>
+        <v>0.10477515000000001</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" si="8"/>
-        <v>0.423871</v>
+        <v>0.30592349999999996</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="8"/>
@@ -1116,19 +1267,40 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>7.8900600000000001E-2</v>
+      </c>
+      <c r="K40">
+        <v>0.37669200000000003</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <f t="shared" ref="B41:H41" si="9">$B$31*B10+(1-$B$31)*B25</f>
-        <v>2.5464275E-4</v>
+        <v>6.4533212500000002E-4</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" si="9"/>
-        <v>3.2999109999999998E-2</v>
+        <v>0.11378318500000001</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="9"/>
-        <v>0.68770825000000002</v>
+        <v>0.40233137499999999</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="9"/>
@@ -1146,27 +1318,48 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>4.1091850000000003E-4</v>
+      </c>
+      <c r="K41">
+        <v>6.5312739999999994E-2</v>
+      </c>
+      <c r="L41">
+        <v>0.57355749999999994</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <f t="shared" ref="B42:H42" si="10">$B$31*B11+(1-$B$31)*B26</f>
-        <v>1.0333145E-6</v>
+        <v>3.29713575E-6</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" si="10"/>
-        <v>1.5585029354624999E-4</v>
+        <v>5.4547504892437499E-4</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="10"/>
-        <v>5.6682599E-2</v>
+        <v>0.19658876650000001</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="10"/>
-        <v>0.45082109999999997</v>
+        <v>0.15099384999999999</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="10"/>
-        <v>6.7026399999999992E-5</v>
+        <v>7.0701899999999995E-5</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="10"/>
@@ -1176,95 +1369,179 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>1.9388430000000001E-6</v>
+      </c>
+      <c r="K42">
+        <v>3.1170019569749997E-4</v>
+      </c>
+      <c r="L42">
+        <v>0.112645066</v>
+      </c>
+      <c r="M42">
+        <v>0.33089020000000002</v>
+      </c>
+      <c r="N42">
+        <v>6.8496599999999991E-5</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <f t="shared" ref="B43:H43" si="11">$B$31*B12+(1-$B$31)*B27</f>
-        <v>1.3296E-8</v>
+        <v>4.6536000000000001E-8</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" si="11"/>
-        <v>1.20005E-5</v>
+        <v>4.2001749999999998E-5</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" si="11"/>
-        <v>4.2497500000000001E-3</v>
+        <v>1.4874125E-2</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="11"/>
-        <v>0.10497261249999999</v>
+        <v>0.36375376875000004</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="11"/>
-        <v>0.190663</v>
+        <v>0.14772550000000001</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="11"/>
-        <v>1.3221275000000002E-3</v>
+        <v>2.0667712500000001E-3</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>2.6592000000000001E-8</v>
+      </c>
+      <c r="K43">
+        <v>2.4000999999999999E-5</v>
+      </c>
+      <c r="L43">
+        <v>8.4995000000000001E-3</v>
+      </c>
+      <c r="M43">
+        <v>0.20848507499999999</v>
+      </c>
+      <c r="N43">
+        <v>0.173488</v>
+      </c>
+      <c r="O43">
+        <v>1.619985E-3</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <f t="shared" ref="B44:H44" si="12">$B$31*B13+(1-$B$31)*B28</f>
         <v>0</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="12"/>
-        <v>1.86215E-6</v>
+        <v>6.5175249999999999E-6</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="12"/>
-        <v>6.6107500000000001E-4</v>
+        <v>2.3137625000000002E-3</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="12"/>
-        <v>1.5932999999999999E-2</v>
+        <v>5.5765499999999996E-2</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="12"/>
-        <v>0.13081614500000002</v>
+        <v>0.44831935750000002</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="12"/>
-        <v>0.32682699999999998</v>
+        <v>0.63773199999999997</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" si="12"/>
-        <v>3.5757822500000001E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.11632630375</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>3.7243000000000001E-6</v>
+      </c>
+      <c r="L44">
+        <v>1.32215E-3</v>
+      </c>
+      <c r="M44">
+        <v>3.1865999999999998E-2</v>
+      </c>
+      <c r="N44">
+        <v>0.25781743000000001</v>
+      </c>
+      <c r="O44">
+        <v>0.45118900000000001</v>
+      </c>
+      <c r="P44">
+        <v>6.7985215000000002E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <f t="shared" ref="B45:H45" si="13">$B$31*B14+(1-$B$31)*B29</f>
         <v>0</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" si="13"/>
-        <v>2.61375E-7</v>
+        <v>9.1481249999999993E-7</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="13"/>
-        <v>1.2585999999999999E-4</v>
+        <v>4.4050999999999997E-4</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="13"/>
-        <v>3.0347500000000001E-3</v>
+        <v>1.0621625000000001E-2</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="13"/>
-        <v>1.5307252773199999E-2</v>
+        <v>5.3575375462200002E-2</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="13"/>
-        <v>0.13789467499999999</v>
+        <v>0.47074911250000001</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="13"/>
-        <v>1.1141227499999999</v>
+        <v>2.2529371250000003</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>5.2274999999999999E-7</v>
+      </c>
+      <c r="L45">
+        <v>2.5171999999999998E-4</v>
+      </c>
+      <c r="M45">
+        <v>6.0695000000000002E-3</v>
+      </c>
+      <c r="N45">
+        <v>3.0614501848799998E-2</v>
+      </c>
+      <c r="O45">
+        <v>0.27103644999999998</v>
+      </c>
+      <c r="P45">
+        <v>1.5696485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>